<commit_message>
Enhance data management: update backup files for Orders, Products, Discounts, and Shopkeepers; modify SQL queries and UI components for improved functionality
</commit_message>
<xml_diff>
--- a/Backup/Khata.xlsx
+++ b/Backup/Khata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,10 +467,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -478,11 +478,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-02-12</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -491,25 +491,61 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Bonapapa</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>14532.068625</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>22</v>
+      </c>
+      <c r="B4" t="n">
+        <v>18</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Candyland</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-02-18</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="D4" t="n">
+        <v>2860560.064569599</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Candyland</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>